<commit_message>
Got full timings for mailslots
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
+    <sheet name="MAILSLOT RESULTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -108,12 +109,30 @@
   <si>
     <t>Data Copy (40 Bytes)</t>
   </si>
+  <si>
+    <t xml:space="preserve">40 BYTES </t>
+  </si>
+  <si>
+    <t>400 BYTES</t>
+  </si>
+  <si>
+    <t>4000 BYTES</t>
+  </si>
+  <si>
+    <t>40 000 BYTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAILSLOTS --&gt; Purely JNI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAILSLOTS --&gt; Java IO Write </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +170,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,12 +206,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -279,7 +318,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -466,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -474,7 +513,7 @@
   <cols>
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1049,4 +1088,461 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>804624</v>
+      </c>
+      <c r="C3">
+        <v>822371</v>
+      </c>
+      <c r="D3">
+        <v>879385</v>
+      </c>
+      <c r="E3">
+        <v>919032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>650949</v>
+      </c>
+      <c r="C4">
+        <v>601108</v>
+      </c>
+      <c r="D4">
+        <v>959810</v>
+      </c>
+      <c r="E4">
+        <v>1089698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>699657</v>
+      </c>
+      <c r="C5">
+        <v>981332</v>
+      </c>
+      <c r="D5">
+        <v>1046654</v>
+      </c>
+      <c r="E5">
+        <v>1041746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>465179</v>
+      </c>
+      <c r="C6">
+        <v>721179</v>
+      </c>
+      <c r="D6">
+        <v>987751</v>
+      </c>
+      <c r="E6">
+        <v>994925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>485191</v>
+      </c>
+      <c r="C7">
+        <v>920164</v>
+      </c>
+      <c r="D7">
+        <v>1055338</v>
+      </c>
+      <c r="E7">
+        <v>966984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>654725</v>
+      </c>
+      <c r="C8">
+        <v>907327</v>
+      </c>
+      <c r="D8">
+        <v>1023999</v>
+      </c>
+      <c r="E8">
+        <v>1061002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>830678</v>
+      </c>
+      <c r="C9">
+        <v>934135</v>
+      </c>
+      <c r="D9">
+        <v>1033438</v>
+      </c>
+      <c r="E9">
+        <v>858241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>546737</v>
+      </c>
+      <c r="C10">
+        <v>899020</v>
+      </c>
+      <c r="D10">
+        <v>864660</v>
+      </c>
+      <c r="E10">
+        <v>1009651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>770642</v>
+      </c>
+      <c r="C11">
+        <v>1082524</v>
+      </c>
+      <c r="D11">
+        <v>944330</v>
+      </c>
+      <c r="E11">
+        <v>809911</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>751008</v>
+      </c>
+      <c r="C12">
+        <v>839740</v>
+      </c>
+      <c r="D12">
+        <v>920542</v>
+      </c>
+      <c r="E12">
+        <v>1081391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7">
+        <f>AVERAGE(B3:B12)</f>
+        <v>665939</v>
+      </c>
+      <c r="C13" s="7">
+        <f>AVERAGE(C3:C12)</f>
+        <v>870890</v>
+      </c>
+      <c r="D13" s="7">
+        <f>AVERAGE(D3:D12)</f>
+        <v>971590.7</v>
+      </c>
+      <c r="E13" s="7">
+        <f>AVERAGE(E3:E12)</f>
+        <v>983258.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>185770</v>
+      </c>
+      <c r="C17">
+        <v>226926</v>
+      </c>
+      <c r="D17">
+        <v>172177</v>
+      </c>
+      <c r="E17">
+        <v>177463</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>194454</v>
+      </c>
+      <c r="C18">
+        <v>216354</v>
+      </c>
+      <c r="D18">
+        <v>324342</v>
+      </c>
+      <c r="E18">
+        <v>234477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>269215</v>
+      </c>
+      <c r="C19">
+        <v>221640</v>
+      </c>
+      <c r="D19">
+        <v>221640</v>
+      </c>
+      <c r="E19">
+        <v>291870</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>178596</v>
+      </c>
+      <c r="C20">
+        <v>231079</v>
+      </c>
+      <c r="D20">
+        <v>178596</v>
+      </c>
+      <c r="E20">
+        <v>206537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>194077</v>
+      </c>
+      <c r="C21">
+        <v>187280</v>
+      </c>
+      <c r="D21">
+        <v>180106</v>
+      </c>
+      <c r="E21">
+        <v>177840</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>224283</v>
+      </c>
+      <c r="C22">
+        <v>229946</v>
+      </c>
+      <c r="D22">
+        <v>217864</v>
+      </c>
+      <c r="E22">
+        <v>213711</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>195964</v>
+      </c>
+      <c r="C23">
+        <v>234478</v>
+      </c>
+      <c r="D23">
+        <v>282430</v>
+      </c>
+      <c r="E23">
+        <v>214088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>236365</v>
+      </c>
+      <c r="C24">
+        <v>238254</v>
+      </c>
+      <c r="D24">
+        <v>179729</v>
+      </c>
+      <c r="E24">
+        <v>411186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>265439</v>
+      </c>
+      <c r="C25">
+        <v>266572</v>
+      </c>
+      <c r="D25">
+        <v>181239</v>
+      </c>
+      <c r="E25">
+        <v>190678</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>184260</v>
+      </c>
+      <c r="C26">
+        <v>166514</v>
+      </c>
+      <c r="D26">
+        <v>303952</v>
+      </c>
+      <c r="E26">
+        <v>203516</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f>AVERAGE(B17:B26)</f>
+        <v>212842.3</v>
+      </c>
+      <c r="C27">
+        <f>AVERAGE(C17:C26)</f>
+        <v>221904.3</v>
+      </c>
+      <c r="D27">
+        <f>AVERAGE(D17:D26)</f>
+        <v>224207.5</v>
+      </c>
+      <c r="E27">
+        <f>AVERAGE(E17:E26)</f>
+        <v>232136.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NPs understand byte array messages. Full timings recorded
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
     <sheet name="MAILSLOT RESULTS" sheetId="2" r:id="rId2"/>
+    <sheet name="NAMED PIPE RESULTS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -126,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAILSLOTS --&gt; Java IO Write </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAMED PIPES </t>
   </si>
 </sst>
 </file>
@@ -209,12 +213,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -223,6 +221,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,26 +522,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -893,16 +897,16 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1094,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,33 +1109,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3">
@@ -1148,7 +1152,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4">
@@ -1165,7 +1169,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5">
@@ -1182,7 +1186,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6">
@@ -1199,7 +1203,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7">
@@ -1216,7 +1220,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8">
@@ -1233,7 +1237,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9">
@@ -1250,7 +1254,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10">
@@ -1267,7 +1271,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1284,7 +1288,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1301,53 +1305,53 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <f>AVERAGE(B3:B12)</f>
         <v>665939</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <f>AVERAGE(C3:C12)</f>
         <v>870890</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <f>AVERAGE(D3:D12)</f>
         <v>971590.7</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <f>AVERAGE(E3:E12)</f>
         <v>983258.1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17">
@@ -1364,7 +1368,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
       <c r="B18">
@@ -1381,7 +1385,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
       <c r="B19">
@@ -1398,7 +1402,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
       <c r="B20">
@@ -1415,7 +1419,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
       <c r="B21">
@@ -1432,7 +1436,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <v>6</v>
       </c>
       <c r="B22">
@@ -1449,7 +1453,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <v>7</v>
       </c>
       <c r="B23">
@@ -1466,7 +1470,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <v>8</v>
       </c>
       <c r="B24">
@@ -1483,7 +1487,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <v>9</v>
       </c>
       <c r="B25">
@@ -1500,7 +1504,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <v>10</v>
       </c>
       <c r="B26">
@@ -1517,7 +1521,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B27">
@@ -1545,4 +1549,240 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>672093</v>
+      </c>
+      <c r="C3">
+        <v>818218</v>
+      </c>
+      <c r="D3">
+        <v>890335</v>
+      </c>
+      <c r="E3">
+        <v>1057604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>773663</v>
+      </c>
+      <c r="C4">
+        <v>1051562</v>
+      </c>
+      <c r="D4">
+        <v>870324</v>
+      </c>
+      <c r="E4">
+        <v>958300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>995681</v>
+      </c>
+      <c r="C5">
+        <v>1053073</v>
+      </c>
+      <c r="D5">
+        <v>835964</v>
+      </c>
+      <c r="E5">
+        <v>637734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1108577</v>
+      </c>
+      <c r="C6">
+        <v>926206</v>
+      </c>
+      <c r="D6">
+        <v>797073</v>
+      </c>
+      <c r="E6">
+        <v>1122925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1071574</v>
+      </c>
+      <c r="C7">
+        <v>842383</v>
+      </c>
+      <c r="D7">
+        <v>1341544</v>
+      </c>
+      <c r="E7">
+        <v>723067</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>680401</v>
+      </c>
+      <c r="C8">
+        <v>1053828</v>
+      </c>
+      <c r="D8">
+        <v>1311338</v>
+      </c>
+      <c r="E8">
+        <v>998324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1064023</v>
+      </c>
+      <c r="C9">
+        <v>761203</v>
+      </c>
+      <c r="D9">
+        <v>714760</v>
+      </c>
+      <c r="E9">
+        <v>1127834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1051940</v>
+      </c>
+      <c r="C10">
+        <v>845781</v>
+      </c>
+      <c r="D10">
+        <v>805002</v>
+      </c>
+      <c r="E10">
+        <v>968117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1041746</v>
+      </c>
+      <c r="C11">
+        <v>1148600</v>
+      </c>
+      <c r="D11">
+        <v>593934</v>
+      </c>
+      <c r="E11">
+        <v>1051562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>618855</v>
+      </c>
+      <c r="C12">
+        <v>941687</v>
+      </c>
+      <c r="D12">
+        <v>807645</v>
+      </c>
+      <c r="E12">
+        <v>1038347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5">
+        <f>AVERAGE(B3:B12)</f>
+        <v>907855.3</v>
+      </c>
+      <c r="C13" s="5">
+        <f>AVERAGE(C3:C12)</f>
+        <v>944254.1</v>
+      </c>
+      <c r="D13" s="5">
+        <f>AVERAGE(D3:D12)</f>
+        <v>896791.9</v>
+      </c>
+      <c r="E13" s="5">
+        <f>AVERAGE(E3:E12)</f>
+        <v>968381.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Winsock understands byte arrays. Full timings collected
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
     <sheet name="MAILSLOT RESULTS" sheetId="2" r:id="rId2"/>
     <sheet name="NAMED PIPE RESULTS" sheetId="3" r:id="rId3"/>
+    <sheet name="WINSOCK RESULTS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -130,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">NAMED PIPES </t>
+  </si>
+  <si>
+    <t>Winsock</t>
   </si>
 </sst>
 </file>
@@ -509,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,4 +1789,242 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2345909</v>
+      </c>
+      <c r="C3">
+        <v>2366676</v>
+      </c>
+      <c r="D3">
+        <v>3408044</v>
+      </c>
+      <c r="E3">
+        <v>40499313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2816752</v>
+      </c>
+      <c r="C4">
+        <v>2796741</v>
+      </c>
+      <c r="D4">
+        <v>2419160</v>
+      </c>
+      <c r="E4">
+        <v>36669511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2543384</v>
+      </c>
+      <c r="C5">
+        <v>2245850</v>
+      </c>
+      <c r="D5">
+        <v>2563396</v>
+      </c>
+      <c r="E5">
+        <v>45141669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2550180</v>
+      </c>
+      <c r="C6">
+        <v>2804670</v>
+      </c>
+      <c r="D6">
+        <v>4356904</v>
+      </c>
+      <c r="E6">
+        <v>40935419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2815242</v>
+      </c>
+      <c r="C7">
+        <v>2389331</v>
+      </c>
+      <c r="D7">
+        <v>2336848</v>
+      </c>
+      <c r="E7">
+        <v>34904321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2815242</v>
+      </c>
+      <c r="C8">
+        <v>2938334</v>
+      </c>
+      <c r="D8">
+        <v>3912114</v>
+      </c>
+      <c r="E8">
+        <v>37184909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2720847</v>
+      </c>
+      <c r="C9">
+        <v>2783526</v>
+      </c>
+      <c r="D9">
+        <v>2057438</v>
+      </c>
+      <c r="E9">
+        <v>47468698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2717071</v>
+      </c>
+      <c r="C10">
+        <v>4036716</v>
+      </c>
+      <c r="D10">
+        <v>2755207</v>
+      </c>
+      <c r="E10">
+        <v>46709384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2689885</v>
+      </c>
+      <c r="C11">
+        <v>2857531</v>
+      </c>
+      <c r="D11">
+        <v>3334794</v>
+      </c>
+      <c r="E11">
+        <v>36363671</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2598511</v>
+      </c>
+      <c r="C12">
+        <v>3857365</v>
+      </c>
+      <c r="D12">
+        <v>3908717</v>
+      </c>
+      <c r="E12">
+        <v>32130990</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5">
+        <f>AVERAGE(B3:B12)</f>
+        <v>2661302.2999999998</v>
+      </c>
+      <c r="C13" s="5">
+        <f>AVERAGE(C3:C12)</f>
+        <v>2907674</v>
+      </c>
+      <c r="D13" s="5">
+        <f>AVERAGE(D3:D12)</f>
+        <v>3105262.2</v>
+      </c>
+      <c r="E13" s="5">
+        <f>AVERAGE(E3:E12)</f>
+        <v>39800788.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Java Sockets understands byte array messages. Timing collected
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
     <sheet name="MAILSLOT RESULTS" sheetId="2" r:id="rId2"/>
     <sheet name="NAMED PIPE RESULTS" sheetId="3" r:id="rId3"/>
     <sheet name="WINSOCK RESULTS" sheetId="4" r:id="rId4"/>
+    <sheet name="JAVA SOCKETS RESULTS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -134,6 +135,9 @@
   </si>
   <si>
     <t>Winsock</t>
+  </si>
+  <si>
+    <t>Java Sockets (No JNI)</t>
   </si>
 </sst>
 </file>
@@ -513,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29:H31"/>
     </sheetView>
   </sheetViews>
@@ -1795,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,4 +2031,242 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5913293</v>
+      </c>
+      <c r="C3">
+        <v>5980502</v>
+      </c>
+      <c r="D3">
+        <v>7009409</v>
+      </c>
+      <c r="E3">
+        <v>6315794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>6116808</v>
+      </c>
+      <c r="C4">
+        <v>6142107</v>
+      </c>
+      <c r="D4">
+        <v>6151546</v>
+      </c>
+      <c r="E4">
+        <v>6184396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>6149657</v>
+      </c>
+      <c r="C5">
+        <v>6368655</v>
+      </c>
+      <c r="D5">
+        <v>6008065</v>
+      </c>
+      <c r="E5">
+        <v>5937080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6090000</v>
+      </c>
+      <c r="C6">
+        <v>6108124</v>
+      </c>
+      <c r="D6">
+        <v>5711664</v>
+      </c>
+      <c r="E6">
+        <v>6934271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6074142</v>
+      </c>
+      <c r="C7">
+        <v>6122472</v>
+      </c>
+      <c r="D7">
+        <v>6719805</v>
+      </c>
+      <c r="E7">
+        <v>5744891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>5859676</v>
+      </c>
+      <c r="C8">
+        <v>5820786</v>
+      </c>
+      <c r="D8">
+        <v>5751310</v>
+      </c>
+      <c r="E8">
+        <v>6995817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>6604642</v>
+      </c>
+      <c r="C9">
+        <v>5925375</v>
+      </c>
+      <c r="D9">
+        <v>6303711</v>
+      </c>
+      <c r="E9">
+        <v>5621799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5592726</v>
+      </c>
+      <c r="C10">
+        <v>5822673</v>
+      </c>
+      <c r="D10">
+        <v>6430200</v>
+      </c>
+      <c r="E10">
+        <v>5738095</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>5438673</v>
+      </c>
+      <c r="C11">
+        <v>6219887</v>
+      </c>
+      <c r="D11">
+        <v>5604431</v>
+      </c>
+      <c r="E11">
+        <v>6887450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>6552159</v>
+      </c>
+      <c r="C12">
+        <v>5653895</v>
+      </c>
+      <c r="D12">
+        <v>6486082</v>
+      </c>
+      <c r="E12">
+        <v>6496654</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>6039177.5999999996</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
+        <v>6016447.5999999996</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>6217622.2999999998</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6285624.7000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MemMap now understands byte arrays. Timings collected
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="NAMED PIPE RESULTS" sheetId="3" r:id="rId3"/>
     <sheet name="WINSOCK RESULTS" sheetId="4" r:id="rId4"/>
     <sheet name="JAVA SOCKETS RESULTS" sheetId="5" r:id="rId5"/>
+    <sheet name="MEM MAP RESULTS" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -2037,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,4 +2270,240 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>106100</v>
+      </c>
+      <c r="C3">
+        <v>106855</v>
+      </c>
+      <c r="D3">
+        <v>103457</v>
+      </c>
+      <c r="E3">
+        <v>81557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>89110</v>
+      </c>
+      <c r="C4">
+        <v>99682</v>
+      </c>
+      <c r="D4">
+        <v>76649</v>
+      </c>
+      <c r="E4">
+        <v>118561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>83823</v>
+      </c>
+      <c r="C5">
+        <v>86089</v>
+      </c>
+      <c r="D5">
+        <v>74761</v>
+      </c>
+      <c r="E5">
+        <v>71363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>71741</v>
+      </c>
+      <c r="C6">
+        <v>74383</v>
+      </c>
+      <c r="D6">
+        <v>350395</v>
+      </c>
+      <c r="E6">
+        <v>131021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>69474</v>
+      </c>
+      <c r="C7">
+        <v>76271</v>
+      </c>
+      <c r="D7">
+        <v>95150</v>
+      </c>
+      <c r="E7">
+        <v>74383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>79292</v>
+      </c>
+      <c r="C8">
+        <v>78537</v>
+      </c>
+      <c r="D8">
+        <v>103079</v>
+      </c>
+      <c r="E8">
+        <v>79291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>118560</v>
+      </c>
+      <c r="C9">
+        <v>152920</v>
+      </c>
+      <c r="D9">
+        <v>103080</v>
+      </c>
+      <c r="E9">
+        <v>72873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>75516</v>
+      </c>
+      <c r="C10">
+        <v>126867</v>
+      </c>
+      <c r="D10">
+        <v>118938</v>
+      </c>
+      <c r="E10">
+        <v>76649</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>79292</v>
+      </c>
+      <c r="C11">
+        <v>72117</v>
+      </c>
+      <c r="D11">
+        <v>86844</v>
+      </c>
+      <c r="E11">
+        <v>79292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>73628</v>
+      </c>
+      <c r="C12">
+        <v>79670</v>
+      </c>
+      <c r="D12">
+        <v>81180</v>
+      </c>
+      <c r="E12">
+        <v>77404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>84653.6</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C3:C12)</f>
+        <v>95339.1</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D3:D12)</f>
+        <v>119353.3</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E3:E12)</f>
+        <v>86239.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data Copy understands byte arrays. Data collected
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="840" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="840"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="WINSOCK RESULTS" sheetId="4" r:id="rId4"/>
     <sheet name="JAVA SOCKETS RESULTS" sheetId="5" r:id="rId5"/>
     <sheet name="MEM MAP RESULTS" sheetId="6" r:id="rId6"/>
+    <sheet name="DATA COPY RESULTS" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="20">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -139,6 +140,9 @@
   </si>
   <si>
     <t>Java Sockets (No JNI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Copy </t>
   </si>
 </sst>
 </file>
@@ -518,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29:H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2043,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,19 +2251,19 @@
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>AVERAGE(B3:B12)</f>
         <v>6039177.5999999996</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f t="shared" ref="C13:E13" si="0">AVERAGE(C3:C12)</f>
         <v>6016447.5999999996</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>6217622.2999999998</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f t="shared" si="0"/>
         <v>6285624.7000000002</v>
       </c>
@@ -2276,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,19 +2487,19 @@
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>AVERAGE(B3:B12)</f>
         <v>84653.6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>AVERAGE(C3:C12)</f>
         <v>95339.1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f>AVERAGE(D3:D12)</f>
         <v>119353.3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f>AVERAGE(E3:E12)</f>
         <v>86239.4</v>
       </c>
@@ -2506,4 +2510,241 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>327736706</v>
+      </c>
+      <c r="C3">
+        <v>1909893371</v>
+      </c>
+      <c r="D3">
+        <v>1908259201</v>
+      </c>
+      <c r="E3">
+        <v>1781589540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3007405114</v>
+      </c>
+      <c r="C4">
+        <v>2582338660</v>
+      </c>
+      <c r="D4">
+        <v>1752484104</v>
+      </c>
+      <c r="E4">
+        <v>1981037516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2001113863</v>
+      </c>
+      <c r="C5">
+        <v>2078005921</v>
+      </c>
+      <c r="D5">
+        <v>1599648095</v>
+      </c>
+      <c r="E5">
+        <v>1675578076</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5738582713</v>
+      </c>
+      <c r="C6">
+        <v>1991966214</v>
+      </c>
+      <c r="D6">
+        <v>1584572805</v>
+      </c>
+      <c r="E6">
+        <v>2259836734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1440270499</v>
+      </c>
+      <c r="C7">
+        <v>1723703388</v>
+      </c>
+      <c r="D7">
+        <v>1612499811</v>
+      </c>
+      <c r="E7">
+        <v>1894197717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1281181753</v>
+      </c>
+      <c r="C8">
+        <v>1638359940</v>
+      </c>
+      <c r="D8">
+        <v>2904203229</v>
+      </c>
+      <c r="E8">
+        <v>2011930042</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2111512815</v>
+      </c>
+      <c r="C9">
+        <v>2371708251</v>
+      </c>
+      <c r="D9">
+        <v>2116357931</v>
+      </c>
+      <c r="E9">
+        <v>4389688270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2074325641</v>
+      </c>
+      <c r="C10">
+        <v>2297538173</v>
+      </c>
+      <c r="D10">
+        <v>2006908595</v>
+      </c>
+      <c r="E10">
+        <v>4113563457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2130233647</v>
+      </c>
+      <c r="C11">
+        <v>1456606153</v>
+      </c>
+      <c r="D11">
+        <v>1624242950</v>
+      </c>
+      <c r="E11">
+        <v>2921578741</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2117753470</v>
+      </c>
+      <c r="C12">
+        <v>1725827280</v>
+      </c>
+      <c r="D12">
+        <v>2629873057</v>
+      </c>
+      <c r="E12">
+        <v>2207160820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5">
+        <f>AVERAGE(B3:B12)</f>
+        <v>2223011622.0999999</v>
+      </c>
+      <c r="C13" s="5">
+        <f>AVERAGE(C3:C12)</f>
+        <v>1977594735.0999999</v>
+      </c>
+      <c r="D13" s="5">
+        <f>AVERAGE(D3:D12)</f>
+        <v>1973904977.8</v>
+      </c>
+      <c r="E13" s="5">
+        <f>AVERAGE(E3:E12)</f>
+        <v>2523616091.3000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created More NP test program
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Message Sent" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sem2" sheetId="2" r:id="rId2"/>
+    <sheet name="Thesis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -148,6 +149,21 @@
   <si>
     <t>0 Bytes</t>
   </si>
+  <si>
+    <t>Named Pipes (JNI Only)</t>
+  </si>
+  <si>
+    <t>Mailslots (Java Write)</t>
+  </si>
+  <si>
+    <t>Named Pipes (Java Write)</t>
+  </si>
+  <si>
+    <t>Named Pipe (JNI Only)</t>
+  </si>
+  <si>
+    <t>Named Pipe (Java Write)</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -223,11 +239,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -235,6 +331,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,7 +421,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Sem2'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -335,7 +442,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Sem2'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -355,7 +462,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>'Sem2'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -385,7 +492,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Sem2'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -406,7 +513,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Sem2'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -426,7 +533,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:f>'Sem2'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -456,7 +563,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Sem2'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -477,7 +584,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Sem2'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -497,7 +604,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>'Sem2'!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -527,7 +634,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'Sem2'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -548,7 +655,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Sem2'!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -568,7 +675,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$5</c:f>
+              <c:f>'Sem2'!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -896,7 +1003,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Sem2'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -917,7 +1024,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'Sem2'!$A$2:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -940,7 +1047,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>'Sem2'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -973,7 +1080,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Sem2'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -994,7 +1101,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'Sem2'!$A$2:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1017,7 +1124,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:f>'Sem2'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1050,7 +1157,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Sem2'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1071,7 +1178,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'Sem2'!$A$2:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1094,7 +1201,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:f>'Sem2'!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1127,7 +1234,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'Sem2'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1148,7 +1255,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>'Sem2'!$A$2:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1171,7 +1278,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$6</c:f>
+              <c:f>'Sem2'!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1564,7 +1671,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Sem2'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1585,7 +1692,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>'Sem2'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1611,7 +1718,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'Sem2'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1647,7 +1754,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Sem2'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1668,7 +1775,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>'Sem2'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1694,7 +1801,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>'Sem2'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1730,7 +1837,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Sem2'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1751,7 +1858,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>'Sem2'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1777,7 +1884,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:f>'Sem2'!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1813,7 +1920,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'Sem2'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1834,7 +1941,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>'Sem2'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1860,7 +1967,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:f>'Sem2'!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2201,7 +2308,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2242,7 +2348,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>'Sem2'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2265,7 +2371,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'Sem2'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2288,7 +2394,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>'Sem2'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2322,7 +2428,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>'Sem2'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2345,7 +2451,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'Sem2'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2368,7 +2474,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>'Sem2'!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2402,7 +2508,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>'Sem2'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2425,7 +2531,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'Sem2'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2448,7 +2554,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>'Sem2'!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2482,7 +2588,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>'Sem2'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2505,7 +2611,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'Sem2'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2528,7 +2634,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$F$5</c:f>
+              <c:f>'Sem2'!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2562,7 +2668,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>'Sem2'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2585,7 +2691,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'Sem2'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2608,7 +2714,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>'Sem2'!$B$8:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2657,7 +2763,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$F$6</c:f>
+              <c:f>'Sem2'!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2808,7 +2914,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2883,7 +2988,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4983,7 +5087,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5571,8 +5675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5773,4 +5877,566 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(C14:C23)</f>
+        <v>83369.899999999994</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE(D14:D23)</f>
+        <v>116974.5</v>
+      </c>
+      <c r="E5">
+        <f>AVERAGE(E14:E23)</f>
+        <v>147143.4</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(F14:F23)</f>
+        <v>235119.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(C25:C34)</f>
+        <v>53087.7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:F6" si="0">AVERAGE(D25:D34)</f>
+        <v>76875.7</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>63546.7</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>107912.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>73628</v>
+      </c>
+      <c r="D14" s="8">
+        <v>104590</v>
+      </c>
+      <c r="E14" s="8">
+        <v>112519</v>
+      </c>
+      <c r="F14" s="9">
+        <v>91752</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>77027</v>
+      </c>
+      <c r="D15" s="8">
+        <v>90242</v>
+      </c>
+      <c r="E15" s="8">
+        <v>106478</v>
+      </c>
+      <c r="F15" s="9">
+        <v>100814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>3</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>74006</v>
+      </c>
+      <c r="D16" s="8">
+        <v>109121</v>
+      </c>
+      <c r="E16" s="8">
+        <v>100814</v>
+      </c>
+      <c r="F16" s="9">
+        <v>580719</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>86466</v>
+      </c>
+      <c r="D17" s="8">
+        <v>75139</v>
+      </c>
+      <c r="E17" s="8">
+        <v>201250</v>
+      </c>
+      <c r="F17" s="9">
+        <v>81558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>74383</v>
+      </c>
+      <c r="D18" s="8">
+        <v>77027</v>
+      </c>
+      <c r="E18" s="8">
+        <v>123847</v>
+      </c>
+      <c r="F18" s="9">
+        <v>877876</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>6</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8">
+        <v>82690</v>
+      </c>
+      <c r="D19" s="8">
+        <v>91374</v>
+      </c>
+      <c r="E19" s="8">
+        <v>148389</v>
+      </c>
+      <c r="F19" s="9">
+        <v>126112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8">
+        <v>87599</v>
+      </c>
+      <c r="D20" s="8">
+        <v>75516</v>
+      </c>
+      <c r="E20" s="8">
+        <v>107611</v>
+      </c>
+      <c r="F20" s="9">
+        <v>80047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>8</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <v>83446</v>
+      </c>
+      <c r="D21" s="8">
+        <v>84200</v>
+      </c>
+      <c r="E21" s="8">
+        <v>300177</v>
+      </c>
+      <c r="F21" s="9">
+        <v>241275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>9</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <v>124224</v>
+      </c>
+      <c r="D22" s="8">
+        <v>367386</v>
+      </c>
+      <c r="E22" s="8">
+        <v>123847</v>
+      </c>
+      <c r="F22" s="9">
+        <v>87599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>10</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11">
+        <v>70230</v>
+      </c>
+      <c r="D23" s="11">
+        <v>95150</v>
+      </c>
+      <c r="E23" s="11">
+        <v>146502</v>
+      </c>
+      <c r="F23" s="12">
+        <v>83445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>1</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8">
+        <v>77782</v>
+      </c>
+      <c r="D25" s="8">
+        <v>67587</v>
+      </c>
+      <c r="E25" s="8">
+        <v>104212</v>
+      </c>
+      <c r="F25" s="9">
+        <v>153676</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0</v>
+      </c>
+      <c r="C26" s="8">
+        <v>44932</v>
+      </c>
+      <c r="D26" s="8">
+        <v>49841</v>
+      </c>
+      <c r="E26" s="8">
+        <v>63433</v>
+      </c>
+      <c r="F26" s="9">
+        <v>123847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>3</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8">
+        <v>48330</v>
+      </c>
+      <c r="D27" s="8">
+        <v>68342</v>
+      </c>
+      <c r="E27" s="8">
+        <v>80047</v>
+      </c>
+      <c r="F27" s="9">
+        <v>95151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>4</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8">
+        <v>66076</v>
+      </c>
+      <c r="D28" s="8">
+        <v>52862</v>
+      </c>
+      <c r="E28" s="8">
+        <v>77026</v>
+      </c>
+      <c r="F28" s="9">
+        <v>92507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>5</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8">
+        <v>58903</v>
+      </c>
+      <c r="D29" s="8">
+        <v>282808</v>
+      </c>
+      <c r="E29" s="8">
+        <v>48331</v>
+      </c>
+      <c r="F29" s="9">
+        <v>125735</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>6</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>45309</v>
+      </c>
+      <c r="D30" s="8">
+        <v>45688</v>
+      </c>
+      <c r="E30" s="8">
+        <v>46820</v>
+      </c>
+      <c r="F30" s="9">
+        <v>84578</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>7</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8">
+        <v>46820</v>
+      </c>
+      <c r="D31" s="8">
+        <v>47953</v>
+      </c>
+      <c r="E31" s="8">
+        <v>45310</v>
+      </c>
+      <c r="F31" s="9">
+        <v>131398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>8</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>44932</v>
+      </c>
+      <c r="D32" s="8">
+        <v>62301</v>
+      </c>
+      <c r="E32" s="8">
+        <v>74383</v>
+      </c>
+      <c r="F32" s="9">
+        <v>109499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>9</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8">
+        <v>52106</v>
+      </c>
+      <c r="D33" s="8">
+        <v>46820</v>
+      </c>
+      <c r="E33" s="8">
+        <v>46064</v>
+      </c>
+      <c r="F33" s="9">
+        <v>86466</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>10</v>
+      </c>
+      <c r="B34" s="11">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11">
+        <v>45687</v>
+      </c>
+      <c r="D34" s="11">
+        <v>44555</v>
+      </c>
+      <c r="E34" s="11">
+        <v>49841</v>
+      </c>
+      <c r="F34" s="12">
+        <v>76271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edited NP Test Programs
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -328,9 +328,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -342,6 +339,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +399,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -816,7 +815,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -864,7 +862,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -961,7 +958,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1429,7 +1425,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1504,7 +1499,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1629,7 +1623,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2121,7 +2114,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2196,7 +2188,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5099,26 +5090,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5474,16 +5465,16 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -5884,7 +5875,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6013,427 +6004,427 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>1</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>0</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>73628</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>104590</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>112519</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>91752</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>0</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>77027</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>90242</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>106478</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>100814</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>3</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>0</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>74006</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>109121</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>100814</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>580719</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>0</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>86466</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>75139</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>201250</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>81558</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>5</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>0</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>74383</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>77027</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>123847</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>877876</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>6</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>0</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>82690</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>91374</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>148389</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>126112</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>7</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>0</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>87599</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>75516</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>107611</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>80047</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>8</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>0</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>83446</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>84200</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>300177</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>241275</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>9</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>0</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>124224</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>367386</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>123847</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>87599</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>10</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>0</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>70230</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <v>95150</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>146502</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="11">
         <v>83445</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>1</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>0</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>77782</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>67587</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>104212</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>153676</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="A26" s="13">
         <v>2</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="7">
         <v>0</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>44932</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>49841</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>63433</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>123847</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
+      <c r="A27" s="13">
         <v>3</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="7">
         <v>0</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>48330</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <v>68342</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>80047</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <v>95151</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="A28" s="13">
         <v>4</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="7">
         <v>0</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>66076</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <v>52862</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <v>77026</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="8">
         <v>92507</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="13">
         <v>5</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>0</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>58903</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <v>282808</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>48331</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="8">
         <v>125735</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="13">
         <v>6</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>0</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>45309</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>45688</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>46820</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="8">
         <v>84578</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>7</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="7">
         <v>0</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>46820</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>47953</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <v>45310</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="8">
         <v>131398</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>8</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>0</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>44932</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>62301</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>74383</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="8">
         <v>109499</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="A33" s="13">
         <v>9</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <v>0</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>52106</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <v>46820</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>46064</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="8">
         <v>86466</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34" s="14">
         <v>10</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="10">
         <v>0</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <v>45687</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <v>44555</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="10">
         <v>49841</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="11">
         <v>76271</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added More MS test programs
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -5872,10 +5872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,6 +5922,22 @@
       <c r="B3">
         <v>0</v>
       </c>
+      <c r="C3">
+        <f>AVERAGE(C36:C45)</f>
+        <v>44441.3</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:F3" si="0">AVERAGE(D36:D45)</f>
+        <v>35115.1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>38286.6</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>67247.199999999997</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5930,6 +5946,22 @@
       <c r="B4">
         <v>0</v>
       </c>
+      <c r="C4">
+        <f>AVERAGE(C47:C56)</f>
+        <v>18274.900000000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:F4" si="1">AVERAGE(D47:D56)</f>
+        <v>19407.8</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>19294.400000000001</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>42893.2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -5967,15 +5999,15 @@
         <v>53087.7</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:F6" si="0">AVERAGE(D25:D34)</f>
+        <f t="shared" ref="D6:F6" si="2">AVERAGE(D25:D34)</f>
         <v>76875.7</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>63546.7</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>107912.8</v>
       </c>
     </row>
@@ -6424,7 +6456,427 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+      <c r="C36" s="7">
+        <v>33227</v>
+      </c>
+      <c r="D36" s="7">
+        <v>46443</v>
+      </c>
+      <c r="E36" s="7">
+        <v>56637</v>
+      </c>
+      <c r="F36" s="8">
+        <v>56637</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>2</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7">
+        <v>32472</v>
+      </c>
+      <c r="D37" s="7">
+        <v>36247</v>
+      </c>
+      <c r="E37" s="7">
+        <v>33604</v>
+      </c>
+      <c r="F37" s="8">
+        <v>56259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>3</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7">
+        <v>84956</v>
+      </c>
+      <c r="D38" s="7">
+        <v>33605</v>
+      </c>
+      <c r="E38" s="7">
+        <v>46820</v>
+      </c>
+      <c r="F38" s="8">
+        <v>56259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>4</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7">
+        <v>32472</v>
+      </c>
+      <c r="D39" s="7">
+        <v>33228</v>
+      </c>
+      <c r="E39" s="7">
+        <v>38513</v>
+      </c>
+      <c r="F39" s="8">
+        <v>75517</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>5</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0</v>
+      </c>
+      <c r="C40" s="7">
+        <v>32095</v>
+      </c>
+      <c r="D40" s="7">
+        <v>33982</v>
+      </c>
+      <c r="E40" s="7">
+        <v>33605</v>
+      </c>
+      <c r="F40" s="8">
+        <v>72118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>6</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7">
+        <v>32472</v>
+      </c>
+      <c r="D41" s="7">
+        <v>33982</v>
+      </c>
+      <c r="E41" s="7">
+        <v>33227</v>
+      </c>
+      <c r="F41" s="8">
+        <v>78537</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>7</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7">
+        <v>33227</v>
+      </c>
+      <c r="D42" s="7">
+        <v>33605</v>
+      </c>
+      <c r="E42" s="7">
+        <v>35870</v>
+      </c>
+      <c r="F42" s="8">
+        <v>73629</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>8</v>
+      </c>
+      <c r="B43" s="7">
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
+        <v>66832</v>
+      </c>
+      <c r="D43" s="7">
+        <v>33227</v>
+      </c>
+      <c r="E43" s="7">
+        <v>34360</v>
+      </c>
+      <c r="F43" s="8">
+        <v>75138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>9</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
+        <v>61545</v>
+      </c>
+      <c r="D44" s="7">
+        <v>33227</v>
+      </c>
+      <c r="E44" s="7">
+        <v>36248</v>
+      </c>
+      <c r="F44" s="8">
+        <v>56260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>10</v>
+      </c>
+      <c r="B45" s="10">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>35115</v>
+      </c>
+      <c r="D45" s="10">
+        <v>33605</v>
+      </c>
+      <c r="E45" s="10">
+        <v>33982</v>
+      </c>
+      <c r="F45" s="11">
+        <v>72118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0</v>
+      </c>
+      <c r="C47" s="7">
+        <v>15858</v>
+      </c>
+      <c r="D47" s="7">
+        <v>16614</v>
+      </c>
+      <c r="E47" s="7">
+        <v>17369</v>
+      </c>
+      <c r="F47" s="8">
+        <v>39646</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>2</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0</v>
+      </c>
+      <c r="C48" s="7">
+        <v>17369</v>
+      </c>
+      <c r="D48" s="7">
+        <v>16614</v>
+      </c>
+      <c r="E48" s="7">
+        <v>31717</v>
+      </c>
+      <c r="F48" s="8">
+        <v>40401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7">
+        <v>0</v>
+      </c>
+      <c r="C49" s="7">
+        <v>15859</v>
+      </c>
+      <c r="D49" s="7">
+        <v>30962</v>
+      </c>
+      <c r="E49" s="7">
+        <v>17369</v>
+      </c>
+      <c r="F49" s="8">
+        <v>40024</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <v>4</v>
+      </c>
+      <c r="B50" s="7">
+        <v>0</v>
+      </c>
+      <c r="C50" s="7">
+        <v>16236</v>
+      </c>
+      <c r="D50" s="7">
+        <v>27940</v>
+      </c>
+      <c r="E50" s="7">
+        <v>16991</v>
+      </c>
+      <c r="F50" s="8">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>5</v>
+      </c>
+      <c r="B51" s="7">
+        <v>0</v>
+      </c>
+      <c r="C51" s="7">
+        <v>17369</v>
+      </c>
+      <c r="D51" s="7">
+        <v>16991</v>
+      </c>
+      <c r="E51" s="7">
+        <v>17368</v>
+      </c>
+      <c r="F51" s="8">
+        <v>54749</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
+        <v>6</v>
+      </c>
+      <c r="B52" s="7">
+        <v>0</v>
+      </c>
+      <c r="C52" s="7">
+        <v>16613</v>
+      </c>
+      <c r="D52" s="7">
+        <v>16614</v>
+      </c>
+      <c r="E52" s="7">
+        <v>17368</v>
+      </c>
+      <c r="F52" s="8">
+        <v>41156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>7</v>
+      </c>
+      <c r="B53" s="7">
+        <v>0</v>
+      </c>
+      <c r="C53" s="7">
+        <v>20011</v>
+      </c>
+      <c r="D53" s="7">
+        <v>17746</v>
+      </c>
+      <c r="E53" s="7">
+        <v>18879</v>
+      </c>
+      <c r="F53" s="8">
+        <v>40024</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <v>8</v>
+      </c>
+      <c r="B54" s="7">
+        <v>0</v>
+      </c>
+      <c r="C54" s="7">
+        <v>17369</v>
+      </c>
+      <c r="D54" s="7">
+        <v>17369</v>
+      </c>
+      <c r="E54" s="7">
+        <v>20767</v>
+      </c>
+      <c r="F54" s="8">
+        <v>38890</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
+        <v>9</v>
+      </c>
+      <c r="B55" s="7">
+        <v>0</v>
+      </c>
+      <c r="C55" s="7">
+        <v>16613</v>
+      </c>
+      <c r="D55" s="7">
+        <v>16614</v>
+      </c>
+      <c r="E55" s="7">
+        <v>17369</v>
+      </c>
+      <c r="F55" s="8">
+        <v>39269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>10</v>
+      </c>
+      <c r="B56" s="10">
+        <v>0</v>
+      </c>
+      <c r="C56" s="10">
+        <v>29452</v>
+      </c>
+      <c r="D56" s="10">
+        <v>16614</v>
+      </c>
+      <c r="E56" s="10">
+        <v>17747</v>
+      </c>
+      <c r="F56" s="11">
+        <v>48708</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Anon Pipes times recorded
</commit_message>
<xml_diff>
--- a/Implementation/TestPrograms/Results/timings.xlsx
+++ b/Implementation/TestPrograms/Results/timings.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -164,6 +164,12 @@
   <si>
     <t>Named Pipe (Java Write)</t>
   </si>
+  <si>
+    <t>Anon Pipes</t>
+  </si>
+  <si>
+    <t>Anonymous Pipes</t>
+  </si>
 </sst>
 </file>
 
@@ -217,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +233,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -342,6 +378,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5872,10 +5913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5916,112 +5957,128 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="18">
         <v>0</v>
       </c>
-      <c r="C3">
-        <f>AVERAGE(C36:C45)</f>
+      <c r="C3" s="18">
+        <f>AVERAGE(C37:C46)</f>
         <v>44441.3</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:F3" si="0">AVERAGE(D36:D45)</f>
+      <c r="D3" s="18">
+        <f t="shared" ref="D3:F3" si="0">AVERAGE(D37:D46)</f>
         <v>35115.1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="18">
         <f t="shared" si="0"/>
         <v>38286.6</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="18">
         <f t="shared" si="0"/>
         <v>67247.199999999997</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="17">
         <v>0</v>
       </c>
-      <c r="C4">
-        <f>AVERAGE(C47:C56)</f>
+      <c r="C4" s="17">
+        <f>AVERAGE(C48:C57)</f>
         <v>18274.900000000001</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:F4" si="1">AVERAGE(D47:D56)</f>
+      <c r="D4" s="17">
+        <f t="shared" ref="D4:F4" si="1">AVERAGE(D48:D57)</f>
         <v>19407.8</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="17">
         <f t="shared" si="1"/>
         <v>19294.400000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="17">
         <f t="shared" si="1"/>
         <v>42893.2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="19">
         <v>0</v>
       </c>
-      <c r="C5">
-        <f>AVERAGE(C14:C23)</f>
+      <c r="C5" s="19">
+        <f>AVERAGE(C15:C24)</f>
         <v>49010.1</v>
       </c>
-      <c r="D5">
-        <f>AVERAGE(D14:D23)</f>
+      <c r="D5" s="19">
+        <f>AVERAGE(D15:D24)</f>
         <v>43686.1</v>
       </c>
-      <c r="E5">
-        <f>AVERAGE(E14:E23)</f>
+      <c r="E5" s="19">
+        <f>AVERAGE(E15:E24)</f>
         <v>59091.6</v>
       </c>
-      <c r="F5">
-        <f>AVERAGE(F14:F23)</f>
+      <c r="F5" s="19">
+        <f>AVERAGE(F15:F24)</f>
         <v>98246.399999999994</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="20">
         <v>0</v>
       </c>
-      <c r="C6">
-        <f>AVERAGE(D25:D34)</f>
+      <c r="C6" s="20">
+        <f>AVERAGE(D26:D35)</f>
         <v>16613.400000000001</v>
       </c>
-      <c r="D6">
-        <f>AVERAGE(C25:C34)</f>
+      <c r="D6" s="20">
+        <f>AVERAGE(C26:C35)</f>
         <v>28922.6</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="D6:F6" si="2">AVERAGE(E25:E34)</f>
+      <c r="E6" s="20">
+        <f t="shared" ref="E6:F6" si="2">AVERAGE(E26:E35)</f>
         <v>50482.5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="20">
         <f t="shared" si="2"/>
         <v>94130.8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="16">
         <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <f>AVERAGE(C59:C68)</f>
+        <v>33264.800000000003</v>
+      </c>
+      <c r="D7" s="16">
+        <f t="shared" ref="D7:F7" si="3">AVERAGE(D59:D68)</f>
+        <v>33869</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="3"/>
+        <v>35530.6</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="3"/>
+        <v>70078.7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6029,497 +6086,485 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>1</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <v>47575</v>
-      </c>
-      <c r="D14" s="7">
-        <v>34360</v>
-      </c>
-      <c r="E14" s="7">
-        <v>37003</v>
-      </c>
-      <c r="F14" s="8">
-        <v>125734</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
       </c>
       <c r="C15" s="7">
-        <v>36626</v>
+        <v>47575</v>
       </c>
       <c r="D15" s="7">
-        <v>41912</v>
+        <v>34360</v>
       </c>
       <c r="E15" s="7">
-        <v>128378</v>
+        <v>37003</v>
       </c>
       <c r="F15" s="8">
-        <v>80424</v>
+        <v>125734</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
       </c>
       <c r="C16" s="7">
-        <v>55505</v>
+        <v>36626</v>
       </c>
       <c r="D16" s="7">
-        <v>89109</v>
+        <v>41912</v>
       </c>
       <c r="E16" s="7">
-        <v>45310</v>
+        <v>128378</v>
       </c>
       <c r="F16" s="8">
-        <v>107610</v>
+        <v>80424</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
       </c>
       <c r="C17" s="7">
-        <v>44554</v>
+        <v>55505</v>
       </c>
       <c r="D17" s="7">
-        <v>32850</v>
+        <v>89109</v>
       </c>
       <c r="E17" s="7">
-        <v>36248</v>
+        <v>45310</v>
       </c>
       <c r="F17" s="8">
-        <v>114407</v>
+        <v>107610</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
       </c>
       <c r="C18" s="7">
-        <v>37381</v>
+        <v>44554</v>
       </c>
       <c r="D18" s="7">
-        <v>38513</v>
+        <v>32850</v>
       </c>
       <c r="E18" s="7">
-        <v>36626</v>
+        <v>36248</v>
       </c>
       <c r="F18" s="8">
-        <v>62301</v>
+        <v>114407</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="7">
         <v>0</v>
       </c>
       <c r="C19" s="7">
-        <v>35870</v>
+        <v>37381</v>
       </c>
       <c r="D19" s="7">
-        <v>44933</v>
+        <v>38513</v>
       </c>
       <c r="E19" s="7">
-        <v>138195</v>
+        <v>36626</v>
       </c>
       <c r="F19" s="8">
-        <v>65700</v>
+        <v>62301</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="7">
         <v>0</v>
       </c>
       <c r="C20" s="7">
-        <v>96283</v>
+        <v>35870</v>
       </c>
       <c r="D20" s="7">
-        <v>36625</v>
+        <v>44933</v>
       </c>
       <c r="E20" s="7">
-        <v>37380</v>
+        <v>138195</v>
       </c>
       <c r="F20" s="8">
-        <v>89109</v>
+        <v>65700</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="7">
         <v>0</v>
       </c>
       <c r="C21" s="7">
-        <v>36248</v>
+        <v>96283</v>
       </c>
       <c r="D21" s="7">
-        <v>33227</v>
+        <v>36625</v>
       </c>
       <c r="E21" s="7">
-        <v>33982</v>
+        <v>37380</v>
       </c>
       <c r="F21" s="8">
-        <v>146878</v>
+        <v>89109</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="7">
         <v>0</v>
       </c>
       <c r="C22" s="7">
+        <v>36248</v>
+      </c>
+      <c r="D22" s="7">
+        <v>33227</v>
+      </c>
+      <c r="E22" s="7">
+        <v>33982</v>
+      </c>
+      <c r="F22" s="8">
+        <v>146878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>9</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
         <v>66454</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D23" s="7">
         <v>33604</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E23" s="7">
         <v>43800</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F23" s="8">
         <v>80425</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
         <v>10</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B24" s="10">
         <v>0</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C24" s="10">
         <v>33605</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D24" s="10">
         <v>51728</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E24" s="10">
         <v>53994</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F24" s="11">
         <v>109876</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
-        <v>20767</v>
-      </c>
-      <c r="D25" s="7">
-        <v>15103</v>
-      </c>
-      <c r="E25" s="7">
-        <v>15103</v>
-      </c>
-      <c r="F25" s="8">
-        <v>123469</v>
-      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="7">
         <v>0</v>
       </c>
       <c r="C26" s="7">
-        <v>30583</v>
+        <v>20767</v>
       </c>
       <c r="D26" s="7">
         <v>15103</v>
       </c>
       <c r="E26" s="7">
-        <v>30962</v>
+        <v>15103</v>
       </c>
       <c r="F26" s="8">
-        <v>99303</v>
+        <v>123469</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="7">
         <v>0</v>
       </c>
       <c r="C27" s="7">
+        <v>30583</v>
+      </c>
+      <c r="D27" s="7">
+        <v>15103</v>
+      </c>
+      <c r="E27" s="7">
         <v>30962</v>
       </c>
-      <c r="D27" s="7">
-        <v>16236</v>
-      </c>
-      <c r="E27" s="7">
-        <v>13971</v>
-      </c>
       <c r="F27" s="8">
-        <v>41156</v>
+        <v>99303</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="7">
         <v>0</v>
       </c>
       <c r="C28" s="7">
-        <v>31339</v>
+        <v>30962</v>
       </c>
       <c r="D28" s="7">
-        <v>13593</v>
+        <v>16236</v>
       </c>
       <c r="E28" s="7">
-        <v>14348</v>
+        <v>13971</v>
       </c>
       <c r="F28" s="8">
-        <v>65321</v>
+        <v>41156</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="7">
         <v>0</v>
       </c>
       <c r="C29" s="7">
-        <v>31716</v>
+        <v>31339</v>
       </c>
       <c r="D29" s="7">
-        <v>15858</v>
+        <v>13593</v>
       </c>
       <c r="E29" s="7">
-        <v>31716</v>
+        <v>14348</v>
       </c>
       <c r="F29" s="8">
-        <v>76649</v>
+        <v>65321</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="7">
         <v>0</v>
       </c>
       <c r="C30" s="7">
-        <v>26809</v>
+        <v>31716</v>
       </c>
       <c r="D30" s="7">
-        <v>13593</v>
+        <v>15858</v>
       </c>
       <c r="E30" s="7">
-        <v>301309</v>
+        <v>31716</v>
       </c>
       <c r="F30" s="8">
-        <v>55504</v>
+        <v>76649</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="7">
         <v>0</v>
       </c>
       <c r="C31" s="7">
-        <v>40401</v>
+        <v>26809</v>
       </c>
       <c r="D31" s="7">
-        <v>14348</v>
+        <v>13593</v>
       </c>
       <c r="E31" s="7">
-        <v>15103</v>
+        <v>301309</v>
       </c>
       <c r="F31" s="8">
-        <v>93640</v>
+        <v>55504</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="7">
         <v>0</v>
       </c>
       <c r="C32" s="7">
-        <v>31339</v>
+        <v>40401</v>
       </c>
       <c r="D32" s="7">
-        <v>33227</v>
+        <v>14348</v>
       </c>
       <c r="E32" s="7">
-        <v>17368</v>
+        <v>15103</v>
       </c>
       <c r="F32" s="8">
-        <v>48331</v>
+        <v>93640</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="7">
         <v>0</v>
       </c>
       <c r="C33" s="7">
+        <v>31339</v>
+      </c>
+      <c r="D33" s="7">
+        <v>33227</v>
+      </c>
+      <c r="E33" s="7">
+        <v>17368</v>
+      </c>
+      <c r="F33" s="8">
+        <v>48331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>9</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0</v>
+      </c>
+      <c r="C34" s="7">
         <v>29829</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D34" s="7">
         <v>14725</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E34" s="7">
         <v>32850</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F34" s="8">
         <v>75139</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>10</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B35" s="10">
         <v>0</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C35" s="10">
         <v>15481</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D35" s="10">
         <v>14348</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E35" s="10">
         <v>32095</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F35" s="11">
         <v>262796</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7">
-        <v>0</v>
-      </c>
-      <c r="C36" s="7">
-        <v>33227</v>
-      </c>
-      <c r="D36" s="7">
-        <v>46443</v>
-      </c>
-      <c r="E36" s="7">
-        <v>56637</v>
-      </c>
-      <c r="F36" s="8">
-        <v>56637</v>
-      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37" s="7">
         <v>0</v>
       </c>
       <c r="C37" s="7">
-        <v>32472</v>
+        <v>33227</v>
       </c>
       <c r="D37" s="7">
-        <v>36247</v>
+        <v>46443</v>
       </c>
       <c r="E37" s="7">
-        <v>33604</v>
+        <v>56637</v>
       </c>
       <c r="F37" s="8">
-        <v>56259</v>
+        <v>56637</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" s="7">
         <v>0</v>
       </c>
       <c r="C38" s="7">
-        <v>84956</v>
+        <v>32472</v>
       </c>
       <c r="D38" s="7">
-        <v>33605</v>
+        <v>36247</v>
       </c>
       <c r="E38" s="7">
-        <v>46820</v>
+        <v>33604</v>
       </c>
       <c r="F38" s="8">
         <v>56259</v>
@@ -6527,356 +6572,581 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" s="7">
         <v>0</v>
       </c>
       <c r="C39" s="7">
-        <v>32472</v>
+        <v>84956</v>
       </c>
       <c r="D39" s="7">
-        <v>33228</v>
+        <v>33605</v>
       </c>
       <c r="E39" s="7">
-        <v>38513</v>
+        <v>46820</v>
       </c>
       <c r="F39" s="8">
-        <v>75517</v>
+        <v>56259</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" s="7">
         <v>0</v>
       </c>
       <c r="C40" s="7">
-        <v>32095</v>
+        <v>32472</v>
       </c>
       <c r="D40" s="7">
-        <v>33982</v>
+        <v>33228</v>
       </c>
       <c r="E40" s="7">
-        <v>33605</v>
+        <v>38513</v>
       </c>
       <c r="F40" s="8">
-        <v>72118</v>
+        <v>75517</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="7">
         <v>0</v>
       </c>
       <c r="C41" s="7">
-        <v>32472</v>
+        <v>32095</v>
       </c>
       <c r="D41" s="7">
         <v>33982</v>
       </c>
       <c r="E41" s="7">
-        <v>33227</v>
+        <v>33605</v>
       </c>
       <c r="F41" s="8">
-        <v>78537</v>
+        <v>72118</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42" s="7">
         <v>0</v>
       </c>
       <c r="C42" s="7">
+        <v>32472</v>
+      </c>
+      <c r="D42" s="7">
+        <v>33982</v>
+      </c>
+      <c r="E42" s="7">
         <v>33227</v>
       </c>
-      <c r="D42" s="7">
-        <v>33605</v>
-      </c>
-      <c r="E42" s="7">
-        <v>35870</v>
-      </c>
       <c r="F42" s="8">
-        <v>73629</v>
+        <v>78537</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" s="7">
         <v>0</v>
       </c>
       <c r="C43" s="7">
-        <v>66832</v>
+        <v>33227</v>
       </c>
       <c r="D43" s="7">
-        <v>33227</v>
+        <v>33605</v>
       </c>
       <c r="E43" s="7">
-        <v>34360</v>
+        <v>35870</v>
       </c>
       <c r="F43" s="8">
-        <v>75138</v>
+        <v>73629</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="7">
         <v>0</v>
       </c>
       <c r="C44" s="7">
-        <v>61545</v>
+        <v>66832</v>
       </c>
       <c r="D44" s="7">
         <v>33227</v>
       </c>
       <c r="E44" s="7">
+        <v>34360</v>
+      </c>
+      <c r="F44" s="8">
+        <v>75138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>9</v>
+      </c>
+      <c r="B45" s="7">
+        <v>0</v>
+      </c>
+      <c r="C45" s="7">
+        <v>61545</v>
+      </c>
+      <c r="D45" s="7">
+        <v>33227</v>
+      </c>
+      <c r="E45" s="7">
         <v>36248</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F45" s="8">
         <v>56260</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
         <v>10</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B46" s="10">
         <v>0</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C46" s="10">
         <v>35115</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D46" s="10">
         <v>33605</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E46" s="10">
         <v>33982</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F46" s="11">
         <v>72118</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="13">
-        <v>1</v>
-      </c>
-      <c r="B47" s="7">
-        <v>0</v>
-      </c>
-      <c r="C47" s="7">
-        <v>15858</v>
-      </c>
-      <c r="D47" s="7">
-        <v>16614</v>
-      </c>
-      <c r="E47" s="7">
-        <v>17369</v>
-      </c>
-      <c r="F47" s="8">
-        <v>39646</v>
-      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" s="7">
         <v>0</v>
       </c>
       <c r="C48" s="7">
-        <v>17369</v>
+        <v>15858</v>
       </c>
       <c r="D48" s="7">
         <v>16614</v>
       </c>
       <c r="E48" s="7">
-        <v>31717</v>
+        <v>17369</v>
       </c>
       <c r="F48" s="8">
-        <v>40401</v>
+        <v>39646</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" s="7">
         <v>0</v>
       </c>
       <c r="C49" s="7">
-        <v>15859</v>
+        <v>17369</v>
       </c>
       <c r="D49" s="7">
-        <v>30962</v>
+        <v>16614</v>
       </c>
       <c r="E49" s="7">
-        <v>17369</v>
+        <v>31717</v>
       </c>
       <c r="F49" s="8">
-        <v>40024</v>
+        <v>40401</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B50" s="7">
         <v>0</v>
       </c>
       <c r="C50" s="7">
-        <v>16236</v>
+        <v>15859</v>
       </c>
       <c r="D50" s="7">
-        <v>27940</v>
+        <v>30962</v>
       </c>
       <c r="E50" s="7">
-        <v>16991</v>
+        <v>17369</v>
       </c>
       <c r="F50" s="8">
-        <v>46065</v>
+        <v>40024</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" s="7">
         <v>0</v>
       </c>
       <c r="C51" s="7">
-        <v>17369</v>
+        <v>16236</v>
       </c>
       <c r="D51" s="7">
+        <v>27940</v>
+      </c>
+      <c r="E51" s="7">
         <v>16991</v>
       </c>
-      <c r="E51" s="7">
-        <v>17368</v>
-      </c>
       <c r="F51" s="8">
-        <v>54749</v>
+        <v>46065</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B52" s="7">
         <v>0</v>
       </c>
       <c r="C52" s="7">
-        <v>16613</v>
+        <v>17369</v>
       </c>
       <c r="D52" s="7">
-        <v>16614</v>
+        <v>16991</v>
       </c>
       <c r="E52" s="7">
         <v>17368</v>
       </c>
       <c r="F52" s="8">
-        <v>41156</v>
+        <v>54749</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" s="7">
         <v>0</v>
       </c>
       <c r="C53" s="7">
-        <v>20011</v>
+        <v>16613</v>
       </c>
       <c r="D53" s="7">
-        <v>17746</v>
+        <v>16614</v>
       </c>
       <c r="E53" s="7">
-        <v>18879</v>
+        <v>17368</v>
       </c>
       <c r="F53" s="8">
-        <v>40024</v>
+        <v>41156</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B54" s="7">
         <v>0</v>
       </c>
       <c r="C54" s="7">
-        <v>17369</v>
+        <v>20011</v>
       </c>
       <c r="D54" s="7">
-        <v>17369</v>
+        <v>17746</v>
       </c>
       <c r="E54" s="7">
-        <v>20767</v>
+        <v>18879</v>
       </c>
       <c r="F54" s="8">
-        <v>38890</v>
+        <v>40024</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" s="7">
         <v>0</v>
       </c>
       <c r="C55" s="7">
+        <v>17369</v>
+      </c>
+      <c r="D55" s="7">
+        <v>17369</v>
+      </c>
+      <c r="E55" s="7">
+        <v>20767</v>
+      </c>
+      <c r="F55" s="8">
+        <v>38890</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
+        <v>9</v>
+      </c>
+      <c r="B56" s="7">
+        <v>0</v>
+      </c>
+      <c r="C56" s="7">
         <v>16613</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D56" s="7">
         <v>16614</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E56" s="7">
         <v>17369</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F56" s="8">
         <v>39269</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="14">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
         <v>10</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B57" s="10">
         <v>0</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C57" s="10">
         <v>29452</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D57" s="10">
         <v>16614</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E57" s="10">
         <v>17747</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F57" s="11">
         <v>48708</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>38136</v>
+      </c>
+      <c r="D59">
+        <v>49085</v>
+      </c>
+      <c r="E59">
+        <v>53995</v>
+      </c>
+      <c r="F59">
+        <v>60035</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>32094</v>
+      </c>
+      <c r="D60">
+        <v>32094</v>
+      </c>
+      <c r="E60">
+        <v>33228</v>
+      </c>
+      <c r="F60">
+        <v>53616</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="13">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>32095</v>
+      </c>
+      <c r="D61">
+        <v>32095</v>
+      </c>
+      <c r="E61">
+        <v>33604</v>
+      </c>
+      <c r="F61">
+        <v>123468</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>28697</v>
+      </c>
+      <c r="D62">
+        <v>31340</v>
+      </c>
+      <c r="E62">
+        <v>33605</v>
+      </c>
+      <c r="F62">
+        <v>52106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>33982</v>
+      </c>
+      <c r="D63">
+        <v>32472</v>
+      </c>
+      <c r="E63">
+        <v>31339</v>
+      </c>
+      <c r="F63">
+        <v>54371</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="13">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>33604</v>
+      </c>
+      <c r="D64">
+        <v>34359</v>
+      </c>
+      <c r="E64">
+        <v>33228</v>
+      </c>
+      <c r="F64">
+        <v>89109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="13">
+        <v>7</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>31339</v>
+      </c>
+      <c r="D65">
+        <v>32472</v>
+      </c>
+      <c r="E65">
+        <v>32849</v>
+      </c>
+      <c r="F65">
+        <v>61923</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13">
+        <v>8</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>38135</v>
+      </c>
+      <c r="D66">
+        <v>30962</v>
+      </c>
+      <c r="E66">
+        <v>32472</v>
+      </c>
+      <c r="F66">
+        <v>85333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="13">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>32850</v>
+      </c>
+      <c r="D67">
+        <v>33227</v>
+      </c>
+      <c r="E67">
+        <v>35493</v>
+      </c>
+      <c r="F67">
+        <v>51729</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>31716</v>
+      </c>
+      <c r="D68">
+        <v>30584</v>
+      </c>
+      <c r="E68">
+        <v>35493</v>
+      </c>
+      <c r="F68">
+        <v>69097</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>